<commit_message>
Added star file to the corpus
</commit_message>
<xml_diff>
--- a/corpus/corpus.xlsx
+++ b/corpus/corpus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MASTER\TMF\Software-Disambiguation\benchmarks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MASTER\TMF\Software-Disambiguation\corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39946D3C-317E-4BA7-9573-D361AFAA1A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BA0BBB-6EC7-42E2-8A44-B68D4F6247C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="597">
   <si>
     <t>id</t>
   </si>
@@ -1164,13 +1164,661 @@
   </si>
   <si>
     <t>Website</t>
+  </si>
+  <si>
+    <t>Spliced Transcripts Alignment to Reference</t>
+  </si>
+  <si>
+    <t>10.7717/peerj.5759</t>
+  </si>
+  <si>
+    <t>Sequences were aligned to the equine genome with Spliced Transcripts Alignment to Reference software</t>
+  </si>
+  <si>
+    <t>Laurence Tessier,Olivier Côté,Dorothee Bienzle</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5074001179,https://openalex.org/A5056307228,https://openalex.org/A5027995244</t>
+  </si>
+  <si>
+    <t>Sanger sequencing,Ensembl,Biology,Genetics,Sequence analysis</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>https://github.com/alexdobin/STAR</t>
+  </si>
+  <si>
+    <t>JelenaDjuric</t>
+  </si>
+  <si>
+    <t>R package STAR</t>
+  </si>
+  <si>
+    <t>10.1016/j.cub.2019.09.005</t>
+  </si>
+  <si>
+    <t>Reads from the RNA-sequencing experiments provided as raw fastq data were quality controlled and mapped to the M. truncatula reference genome version 4.0 (Mt4.0v1) [70] using R package STAR [61]</t>
+  </si>
+  <si>
+    <t>Katharina Schiessl,Jodi L. Stewart Lilley,Tak Lee,Ioannis Tamvakis,Wouter Kohlen,Paul Bailey,Aaron Thomas,Jakub Lupták,Ramakrishnan Karunakaran,Matthew D. Carpenter,Kirankumar S. Mysore,Jiangqi Wen,Sebastian E. Ahnert,Verônica A. Grieneisen,Giles Oldroyd</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5019330809,https://openalex.org/A5004606083,https://openalex.org/A5046964118,https://openalex.org/A5032540563,https://openalex.org/A5037051244,https://openalex.org/A5059141693,https://openalex.org/A5069643039,https://openalex.org/A5047139329,https://openalex.org/A5002054972,https://openalex.org/A5041355825,https://openalex.org/A5003679682,https://openalex.org/A5062304588,https://openalex.org/A5068484674,https://openalex.org/A5023714747,https://openalex.org/A5015269349</t>
+  </si>
+  <si>
+    <t>Biology,Medicago truncatula,Lateral root,Symbiosis,Root nodule,Auxin,Cytokinin,Root hair,Nod factor,Lotus japonicus,Rhizobia,Nodule (geology),Cell biology</t>
+  </si>
+  <si>
+    <t>STAR</t>
+  </si>
+  <si>
+    <t>10.1186/s13568-020-01170-9</t>
+  </si>
+  <si>
+    <t>Sequences were aligned using STAR (Dobin et al</t>
+  </si>
+  <si>
+    <t>B. G. Paes,Andrei Stecca Steindorff,Eduardo Fernandes Formighieri,Ildinete Silva Pereira,J. R. M. de Almeida</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5087399579,https://openalex.org/A5014968407,https://openalex.org/A5088842425,https://openalex.org/A5001590873,https://openalex.org/A5086019850</t>
+  </si>
+  <si>
+    <t>Pichia pastoris,Yeast,Hydrolysate,Biochemistry,Furfural</t>
+  </si>
+  <si>
+    <t>10.1063/5.0054639</t>
+  </si>
+  <si>
+    <t>Analysis was conducted using STAR, R, DeSeq2, and python software.</t>
+  </si>
+  <si>
+    <t>Evan L. Teng,Evan Masutani,Benjamin Yeoman,Jessica Fung,Rachel Lian,Brenda Ngo,Aditya Kumar,Jesse K. Placone,Valentina Lo Sardo,Adam J. Engler</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5086782018,https://openalex.org/A5059609053,https://openalex.org/A5032272935,https://openalex.org/A5075875989,https://openalex.org/A5064632542,https://openalex.org/A5064900633,https://openalex.org/A5003559800,https://openalex.org/A5086699418,https://openalex.org/A5067042085,https://openalex.org/A5039405858</t>
+  </si>
+  <si>
+    <t>Haplotype,Biology,Single-nucleotide polymorphism</t>
+  </si>
+  <si>
+    <t>10.1177/1759091415593066</t>
+  </si>
+  <si>
+    <t>Reads were aligned with the STAR (Dobin et al., 2013) aligner with the additional options (–outFilterMatchNmin 30 –outFilterMismatchNmax 5 –outFilterMismatchNoverLmax 0.05 –outFilterMultimapNmax 50)</t>
+  </si>
+  <si>
+    <t>Frédéric Lebrun-Julien,Ueli Suter</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5060654388,https://openalex.org/A5018900180</t>
+  </si>
+  <si>
+    <t>HDAC1,Neuroprotection,Histone deacetylase 2,Cell biology,Acetylation,Retinal ganglion cell,Biology,Histone deacetylase</t>
+  </si>
+  <si>
+    <t>10.1177/1759091419843393</t>
+  </si>
+  <si>
+    <t>All RNA reads were first mapped to the mouse (GRCm38) reference genome using STAR v2.5.2b release with default parameters (Dobin et al., 2013)</t>
+  </si>
+  <si>
+    <t>Miriam S. Domowicz,Wen-Ching Chan,Patricia Claudio-Vázquez,Judith Henry,Christopher B. Ware,Jorge Andrade,Glyn Dawson,Nancy B. Schwartz</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5038564038,https://openalex.org/A5081364865,https://openalex.org/A5050095889,https://openalex.org/A5014473848,https://openalex.org/A5081683884,https://openalex.org/A5006838633,https://openalex.org/A5054110947,https://openalex.org/A5053781253</t>
+  </si>
+  <si>
+    <t>Forebrain,Biology,Transcriptome,Downregulation and upregulation,Cerebellum</t>
+  </si>
+  <si>
+    <t>10.1107/S2059798321001856</t>
+  </si>
+  <si>
+    <t>Starting with RELION version 3.1, information about optics groups has been added as a second data table to STAR files</t>
+  </si>
+  <si>
+    <t>Grigory Sharov,Dustin R. Morado,Marta Carroni,J.M. de la Rosa-Trevín</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5026727795,https://openalex.org/A5060770584,https://openalex.org/A5089155180,https://openalex.org/A5089413306</t>
+  </si>
+  <si>
+    <t>Plug-in,Computer science,Software,Modular design,Pipeline (software),Flexibility (engineering),Software engineering,Key (lock)</t>
+  </si>
+  <si>
+    <t>STAR package</t>
+  </si>
+  <si>
+    <t>10.1186/s12920-021-01041-7</t>
+  </si>
+  <si>
+    <t>Read quantification was conducted and aligned to the GENCODE v28 (HG38) reference genome using STAR package [16]</t>
+  </si>
+  <si>
+    <t>Ranjit S. Pelia,Suresh Venkateswaran,Jonathan Matthews,Yael Haberman,David J. Cutler,Jeffrey S. Hyams,Lee A. Denson,Subra Kugathasan</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5041038540,https://openalex.org/A5001347503,https://openalex.org/A5046682255,https://openalex.org/A5064124612,https://openalex.org/A5006598488,https://openalex.org/A5006726610,https://openalex.org/A5037750455,https://openalex.org/A5086034125</t>
+  </si>
+  <si>
+    <t>Non-coding RNA,Inflammatory bowel disease,Disease,Epigenetics,Biology,Fold change</t>
+  </si>
+  <si>
+    <t>10.1186/s13059-021-02364-5</t>
+  </si>
+  <si>
+    <t>In brief, STARsolo from STAR package v2.7.5c [14] and Cell Ranger v2.1.1 and scSNV were limited to at most 24 threads</t>
+  </si>
+  <si>
+    <t>Gavin Wilson,Mathieu Derouet,Gail Darling,Jonathan C. Yeung</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5082524303,https://openalex.org/A5035902940,https://openalex.org/A5056959902,https://openalex.org/A5040890688</t>
+  </si>
+  <si>
+    <t>Biology,Computational biology,RNA-Seq,Human genetics,Pipeline (software)</t>
+  </si>
+  <si>
+    <t>star</t>
+  </si>
+  <si>
+    <t>10.1111/acel.12739</t>
+  </si>
+  <si>
+    <t>Illumina sequencing reads were mapped to the annotated Mlig_3_7 genome assembly (Wudarski et al., 2017) using star v.2.5.2b (Dobin et al., 2013) in the transcriptome quantification mode with following parameters “–outFilterMultimapNmax 30 –outFilterMismatchNmax 5 –quantMode TranscriptomeSAM.” To generate read counts for transcript clusters, the resulting bam files were processed by Corset v.1.06 (Davidson &amp; Oshlack, 2014)</t>
+  </si>
+  <si>
+    <t>Stijn Mouton,Magda Grudniewska,Lisa Glazenburg,Victor Guryev,Eugène Berezikov</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5013933341,https://openalex.org/A5054508383,https://openalex.org/A5016131726,https://openalex.org/A5050979301,https://openalex.org/A5008179774</t>
+  </si>
+  <si>
+    <t>Flatworm,Biology,Regeneration (biology),Germline,Caenorhabditis elegans</t>
+  </si>
+  <si>
+    <t>Annotated genomes were retrieved from Ensembl, and RNA‐seq data were mapped and quantified using star v.2.5.2b (Dobin et al., 2013).</t>
+  </si>
+  <si>
+    <t>10.1186/s13015-016-0068-6</t>
+  </si>
+  <si>
+    <t>Suffix arrays are used in such programs as segemehl [3], last [4], mummer [5], reputer [6], star [7], and as an initial stage in recent versions of gsnap [8], which also employs hash tables for more complex alignments.</t>
+  </si>
+  <si>
+    <t>Thomas D. Wu</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5022934719</t>
+  </si>
+  <si>
+    <t>Suffix array,Compressed suffix array,Computer science,Search engine indexing,String (physics),Byte,Suffix,Generalized suffix tree,Genome,Character (mathematics)</t>
+  </si>
+  <si>
+    <t>10.1186/s12885-017-3237-1</t>
+  </si>
+  <si>
+    <t>Raw fastq files were obtained for each sample and aligned to the Homo sapiens reference using star [12]</t>
+  </si>
+  <si>
+    <t>Bojana Jovanović,Quanhu Sheng,Robert S. Seitz,Kasey Lawrence,Stephan W. Morris,Lance R. Thomas,David R. Hout,Brock L. Schweitzer,Yan Guo,Jennifer A. Pietenpol,Brian D. Lehmann</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5031509981,https://openalex.org/A5040171040,https://openalex.org/A5033135467,https://openalex.org/A5057679820,https://openalex.org/A5006599402,https://openalex.org/A5030413393,https://openalex.org/A5075717157,https://openalex.org/A5010230522,https://openalex.org/A5056796466,https://openalex.org/A5032756469,https://openalex.org/A5072853514</t>
+  </si>
+  <si>
+    <t>Subtyping,Triple-negative breast cancer,Concordance,Breast cancer,RNA,Biology</t>
+  </si>
+  <si>
+    <t>10.1186/s12920-021-01022-w</t>
+  </si>
+  <si>
+    <t>After quality control and trimming, the reads were mapped to the human genome (ENSEMBL-grch38release 91) using the star version 2.5.2a aligner and gene abundance was estimated with python version 2.7.11, and htseq version 0.11.0</t>
+  </si>
+  <si>
+    <t>Johanna Bensalel,Hongyuan Xu,Michael L. Lu,Enrico Capobianco,Jianning Wei</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5026065810,https://openalex.org/A5006823789,https://openalex.org/A5039806235,https://openalex.org/A5087254915,https://openalex.org/A5048325890</t>
+  </si>
+  <si>
+    <t>Biology,Huntingtin,Transcriptome,Gene,Genetics</t>
+  </si>
+  <si>
+    <t>10.1099/mgen.0.000319</t>
+  </si>
+  <si>
+    <t>grubii H99 (CNA3, GCA_000149245.3) [22] or Bt85 (Cryp_neof_Bt85_V1, GCA_002215835.1) [16] genome using star (v 2.5.3a) [23] for RNA-Seq mapping, following ‘Alternate Protocol 7’ for star alignment with transcript coordinate output and with rsem (v1.2.31) quantification [24]</t>
+  </si>
+  <si>
+    <t>Yu Chen,Chen Yuan,Christopher A. Desjardins,Jennifer L. Tenor,Dena L. Toffaletti,Charles Giamberardino,Anastasia P. Litvintseva,John R. Perfect,Christina A. Cuomo</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5061166006,https://openalex.org/A5045483608,https://openalex.org/A5070261986,https://openalex.org/A5061409450,https://openalex.org/A5050057628,https://openalex.org/A5007747543,https://openalex.org/A5089720853,https://openalex.org/A5028777325,https://openalex.org/A5009421399</t>
+  </si>
+  <si>
+    <t>Biology,Cryptococcus neoformans,Gene expression,Gene,Transcriptome,Pathogenic fungus</t>
+  </si>
+  <si>
+    <t>STAR RNA-seq aligner package</t>
+  </si>
+  <si>
+    <t>10.1371/journal.pone.0239938</t>
+  </si>
+  <si>
+    <t>taurus UMD 3.1.1) [35] obtained from Ensembl [36] using the STAR RNA-seq aligner package (version 2.5.3a) [37]</t>
+  </si>
+  <si>
+    <t>Jayne E Wiarda,Paola M. Boggiatto,Darrell O. Bayles,W. Ray Waters,Tyler C. Thacker,Mitchell V. Palmer</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5045187716,https://openalex.org/A5020426067,https://openalex.org/A5043932347,https://openalex.org/A5076034149,https://openalex.org/A5076515072,https://openalex.org/A5007656234</t>
+  </si>
+  <si>
+    <t>Biology,Mycobacterium bovis,Immune system,Innate immune system,Transcriptome,Tuberculosis,Immunology,Disease</t>
+  </si>
+  <si>
+    <t>DNA STAR package</t>
+  </si>
+  <si>
+    <t>10.1186/1471-2148-14-143</t>
+  </si>
+  <si>
+    <t>Forward and reverse sequences were assembled and edited with SeqMan (DNA STAR package; DNAStar Inc., Madison, WI, USA).</t>
+  </si>
+  <si>
+    <t>Qing Cai,R. E. Tulloss,Li Tang,Tolgor Bau,Ping Zhang,Zuo H. Chen,Zhu L. Yang</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5058116055,https://openalex.org/A5031893234,https://openalex.org/A5015153358,https://openalex.org/A5046455591,https://openalex.org/A5045479445,https://openalex.org/A5079652183,https://openalex.org/A5065182819</t>
+  </si>
+  <si>
+    <t>Biology,Monophyly,Synapomorphy,Biogeography,Phylogenetic tree</t>
+  </si>
+  <si>
+    <t>https://www.dnastar.com/</t>
+  </si>
+  <si>
+    <t>10.3897/phytokeys.96.23470</t>
+  </si>
+  <si>
+    <t>Sequences were assembled and edited with SeqMan (DNA STAR package; DNA StarInc., Madison, WI, USA), aligned by Bio Edit (Hall 1999) and adjusted manually where necessary</t>
+  </si>
+  <si>
+    <t>Morigengaowa,Jianxun Luo,R. Knapp,Hong‐Jin Wei,Baodong Liu,Yue‐Hong Yan,Hui Shang</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5019857507,https://openalex.org/A5088282123,https://openalex.org/A5023231396,https://openalex.org/A5060654286,https://openalex.org/A5004551670,https://openalex.org/A5043818829,https://openalex.org/A5054476231</t>
+  </si>
+  <si>
+    <t>Herbarium,Synonym (taxonomy),DNA barcoding,Morphology (biology),Biology,Phylogenetic tree</t>
+  </si>
+  <si>
+    <t>10.1371/journal.pone.0026543</t>
+  </si>
+  <si>
+    <t>Neighbor Joining (NJ) tree were constructed using ClustalX protocol from the DNA STAR package</t>
+  </si>
+  <si>
+    <t>Daniela Häming,Marcos Simões-Costa,Benjamin R. Uy,Jonathan E. Valencia,Tatjana Sauka‐Spengler,Marianne Bronner‐Fraser</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5016789606,https://openalex.org/A5082550238,https://openalex.org/A5023202017,https://openalex.org/A5055158439,https://openalex.org/A5058098434,https://openalex.org/A5019521298</t>
+  </si>
+  <si>
+    <t>Lamprey,Neural crest,Biology,Vertebrate,Neural tube,Neuroscience,Chordate,Anatomy</t>
+  </si>
+  <si>
+    <t>10.1371/journal.pone.0175338</t>
+  </si>
+  <si>
+    <t>Forward and reverse sequence chromatograms at each locus were assembled and checked for signal quality using SeqMan (DNA STAR package, DNAStar Inc., Madison, WI, USA)</t>
+  </si>
+  <si>
+    <t>Aisuo Wang,David Gopurenko,Hanwen Wu,Brendan J. Lepschi</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5072657352,https://openalex.org/A5089038469,https://openalex.org/A5073118453,https://openalex.org/A5010802601</t>
+  </si>
+  <si>
+    <t>Biology,DNA barcoding,Invasive species,Weed</t>
+  </si>
+  <si>
+    <t>10.3390/ijms13078740</t>
+  </si>
+  <si>
+    <t>Sequences were assembled and edited using SeqMan (DNA STAR package, DNAStar Inc., Madison, WI, USA)</t>
+  </si>
+  <si>
+    <t>Jie Liu,Jim Provan,Lian‐Ming Gao,De-Zhui Li</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5085352453,https://openalex.org/A5045326231,https://openalex.org/A5028652883,https://openalex.org/A5002089892</t>
+  </si>
+  <si>
+    <t>Indel,DNA barcoding,Biology,Population,Sampling (signal processing),Taxon,Evolutionary biology,Monophyly</t>
+  </si>
+  <si>
+    <t>Spliced Transcripts Alignment to a Reference (STAR)</t>
+  </si>
+  <si>
+    <t>10.1186/s40478-018-0519-z</t>
+  </si>
+  <si>
+    <t>Sequencing raw reads were mapped to the Ensemble RN5 genome with Spliced Transcripts Alignment to a Reference (STAR) software (version 2.3.0e_r291) [24] with parameter alignIntronMax 1 to prohibit splicing and allow genomic mapping</t>
+  </si>
+  <si>
+    <t>Anssi Lipponen,Assam El‐Osta,Antony Kaspi,Mark Ziemann,Ishant Khurana,K N Harikrishnan,Vicente Navarro-Ferrandis,Noora Puhakka,Jussi Paananen,Asla Pitkänen</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5051493682,https://openalex.org/A5025532964,https://openalex.org/A5059094848,https://openalex.org/A5017271798,https://openalex.org/A5045775423,https://openalex.org/A5074902769,https://openalex.org/A5040593045,https://openalex.org/A5066663995,https://openalex.org/A5047977221,https://openalex.org/A5091914497</t>
+  </si>
+  <si>
+    <t>DNA methylation,Transcription factor,Transcriptome,PAX6,Traumatic brain injury</t>
+  </si>
+  <si>
+    <t>10.1186/s40478-016-0338-z</t>
+  </si>
+  <si>
+    <t>For this analysis, we directly aligned all reads from these datasets to an alignment index containing the human genome plus a library of 740 virus genomes (including sequences from all known human viruses documented by NCBI) using the Spliced Transcripts Alignment to a Reference (STAR) aligner</t>
+  </si>
+  <si>
+    <t>Michael J. Strong,Eugene Blanchard,Zhen Lin,Cindy A. Morris,Melody Baddoo,Christopher M. Taylor,Marcus L. Ware,Erik K. Flemington</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5053490217,https://openalex.org/A5023422166,https://openalex.org/A5084051442,https://openalex.org/A5077402829,https://openalex.org/A5089449964,https://openalex.org/A5088041804,https://openalex.org/A5074051253,https://openalex.org/A5002551784</t>
+  </si>
+  <si>
+    <t>Deep sequencing,DNA sequencing,Computational biology,Human virome,Biology</t>
+  </si>
+  <si>
+    <t>10.18632/aging.102840</t>
+  </si>
+  <si>
+    <t>Reads were aligned to the Human reference genome (GRCh37) using the Spliced Transcripts Alignment to a Reference (STAR) software v2.5 [47], then summarized as gene-level counts using featureCounts 1.4.4 [48]</t>
+  </si>
+  <si>
+    <t>Ignazio S. Piras,Christiane Bleul,Joshua S. Talboom,Matthew De Both,Isabelle Schrauwen,Glenda M. Halliday,Amanda Myers,Geidy E. Serrano,Thomas G. Beach,Matthew J. Huentelman</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5081542125,https://openalex.org/A5047225720,https://openalex.org/A5015978195,https://openalex.org/A5001700176,https://openalex.org/A5036840732,https://openalex.org/A5047141421,https://openalex.org/A5021195592,https://openalex.org/A5050607848,https://openalex.org/A5072613176,https://openalex.org/A5037628555</t>
+  </si>
+  <si>
+    <t>Cell type,Biology,Gene expression,Gene</t>
+  </si>
+  <si>
+    <t>10.18632/aging.102968</t>
+  </si>
+  <si>
+    <t>The reads were aligned to the UCSC reference human genome 19 (hg19) using Spliced Transcripts Alignment to a Reference (STAR) software v2.3.1 (DNASTAR, Inc</t>
+  </si>
+  <si>
+    <t>Jian Zhang,Tao Xie,Xi Zhong,Huali Jiang,Rong Li,Baiyao Wang,Xiaoting Huang,Bohong Cen,Yawei Yuan</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5057209439,https://openalex.org/A5063855097,https://openalex.org/A5037099047,https://openalex.org/A5064380788,https://openalex.org/A5042275051,https://openalex.org/A5091395657,https://openalex.org/A5020232250,https://openalex.org/A5001741661,https://openalex.org/A5056810676</t>
+  </si>
+  <si>
+    <t>Nasopharyngeal carcinoma,Wnt signaling pathway,Melatonin,Cisplatin,Cancer research,Catenin,Signal transduction</t>
+  </si>
+  <si>
+    <t>10.3390/ani11041131</t>
+  </si>
+  <si>
+    <t>The clean reads were mapped to the unigenes from full-length transcriptome by Spliced Transcripts Alignment to a Reference (STAR) [26].</t>
+  </si>
+  <si>
+    <t>Xinghua Lin,Dayan Zhou,Xiaomin Zhang,Guangli Li,Yulei Zhang,Cailin Huang,Zhixin Zhang,Changxu Tian</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5051160500,https://openalex.org/A5087290644,https://openalex.org/A5010015600,https://openalex.org/A5004017901,https://openalex.org/A5077811785,https://openalex.org/A5008346736,https://openalex.org/A5021901509,https://openalex.org/A5029462795</t>
+  </si>
+  <si>
+    <t>Catfish,Biology,KEGG,Transcriptome,Danio,Gene</t>
+  </si>
+  <si>
+    <t>10.1186/s12915-016-0279-9</t>
+  </si>
+  <si>
+    <t>Reads were subsequently mapped with Spliced Transcripts Alignment to a Reference (STAR) [92], and gene expression analysis was carried out using HTSeq [93] and DESeq2 [94] with conditional quantile normalization [95]</t>
+  </si>
+  <si>
+    <t>Georg M. Bruun,Thomas Koed Doktor,Jonas Borch-Jensen,Akio Matsubara,Adrian R. Krainer,Kinji Ohno,Brage S. Andresen</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5046162654,https://openalex.org/A5015256307,https://openalex.org/A5028106202,https://openalex.org/A5038516654,https://openalex.org/A5029149817,https://openalex.org/A5017751776,https://openalex.org/A5001821816</t>
+  </si>
+  <si>
+    <t>RNA splicing,Biology,Exon,Splice site mutation,Genetics,Alternative splicing,Intron,Exon skipping,Binding site,Minigene</t>
+  </si>
+  <si>
+    <t>(STAR</t>
+  </si>
+  <si>
+    <t>10.3389/fphys.2020.623190</t>
+  </si>
+  <si>
+    <t>Next, the two reads per sample (R1 and R2) were mapped to the mouse reference genome (build GRCm38/mm10) using Spliced Transcripts Alignment to a Reference (STAR version 2.6.1) (Dobin et al., 2013)</t>
+  </si>
+  <si>
+    <t>Marta Pérez-Hernández,Grecia M Marrón-Liñares,Florencia Schlamp,Adriana Heguy,Chantal J.M. van Opbergen,Valeria Mezzano,Mingliang Zhang,Feng-Xia Liang,Marina Cerrone,Mario Delmar</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5059033144,https://openalex.org/A5079681851,https://openalex.org/A5077847735,https://openalex.org/A5025018584,https://openalex.org/A5029872038,https://openalex.org/A5068456606,https://openalex.org/A5019968053,https://openalex.org/A5045910514,https://openalex.org/A5033233937,https://openalex.org/A5051953374</t>
+  </si>
+  <si>
+    <t>Transcriptome,Myocyte,Biology,Inflammation</t>
+  </si>
+  <si>
+    <t>10.1038/s41598-021-86032-5</t>
+  </si>
+  <si>
+    <t>Then, the high-quality reads were aligned to the reference genome (hg19) using Spliced Transcripts Alignment to a Reference (STAR) with the parameter –quantMode GeneCounts for gene-level quantification and otherwise default parameters</t>
+  </si>
+  <si>
+    <t>Timothy Warwick,Marcel H. Schulz,Stefan Günther,Ralf Gilsbach,Antonio Neme,Carsten Carlberg,Ralf P. Brandes,Sabine Seuter</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5038321079,https://openalex.org/A5080725960,https://openalex.org/A5038168057,https://openalex.org/A5024297412,https://openalex.org/A5023915084,https://openalex.org/A5035613777,https://openalex.org/A5082251197,https://openalex.org/A5010029002</t>
+  </si>
+  <si>
+    <t>Calcitriol receptor,Transcription factor,Biology,Transcriptome,ETS1</t>
+  </si>
+  <si>
+    <t>stars</t>
+  </si>
+  <si>
+    <t>10.1186/s12915-021-01043-y</t>
+  </si>
+  <si>
+    <t>Segmentation maps were converted to polygons in R using packages sf [9] and stars [24]</t>
+  </si>
+  <si>
+    <t>Matthijs J.D. Baars,Neeraj Sinha,Mojtaba Amini,Annelies Pieterman-Bos,Stephanie van Dam,Maroussia M. P. Ganpat,Miangela M. Laclé,Bas Oldenburg,Yvonne Vercoulen</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5044592324,https://openalex.org/A5036518137,https://openalex.org/A5009002591,https://openalex.org/A5012598255,https://openalex.org/A5064177146,https://openalex.org/A5055046375,https://openalex.org/A5047767370,https://openalex.org/A5011860225,https://openalex.org/A5074498599</t>
+  </si>
+  <si>
+    <t>Segmentation,Multiplex,Mass cytometry,Biology</t>
+  </si>
+  <si>
+    <t>https://r-spatial.github.io/stars/,https://cran.r-project.org/package=stars</t>
+  </si>
+  <si>
+    <t>10.1371/journal.pone.0247535</t>
+  </si>
+  <si>
+    <t>The foot package is coded entirely in the R statistical computing language, making use of the sf, stars, and lwgeom packages [27–29] to access external spatial data libraries.</t>
+  </si>
+  <si>
+    <t>Warren C. Jochem,Andrew J. Tatem</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5013702813,https://openalex.org/A5026395399</t>
+  </si>
+  <si>
+    <t>Footprint,Raster graphics,Zoning,Computer science,Scale (ratio)</t>
+  </si>
+  <si>
+    <t>10.1371/journal.pone.0253148</t>
+  </si>
+  <si>
+    <t>All statistical analyses were performed using R [39], and in addition to the packages mentioned previously, we used ggspatial [52], ggplot2 [53], stars [54], tidyverse [55], viridis [56].</t>
+  </si>
+  <si>
+    <t>Julia Carolina Mata,Robert Buitenwerf,Jens‐Christian Svenning</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5079982401,https://openalex.org/A5024327010,https://openalex.org/A5073110322</t>
+  </si>
+  <si>
+    <t>Wildlife,Habitat,Ecology,Restoration ecology,Geography</t>
+  </si>
+  <si>
+    <t>10.1371/journal.pone.0258031</t>
+  </si>
+  <si>
+    <t>We used publicly available packages for the statistical software R (version 4.0.0) [62] and packages tidyverse, PropCIs, ggmap, sf, stars, raster, akima, and adehabitatHR to conduct our GIS and statistical analyses</t>
+  </si>
+  <si>
+    <t>Ryan Takeshita,Brian C. Balmer,Francesca Messina,Eric S. Zolman,Len Thomas,Randall S. Wells,Cynthia R. Smith,Teresa K. Rowles,Lori H. Schwacke</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5037799026,https://openalex.org/A5068536572,https://openalex.org/A5044513551,https://openalex.org/A5051585211,https://openalex.org/A5053540460,https://openalex.org/A5020743541,https://openalex.org/A5038634412,https://openalex.org/A5049890809,https://openalex.org/A5015313746</t>
+  </si>
+  <si>
+    <t>Salinity,Estuary,Bay</t>
+  </si>
+  <si>
+    <t>10.3390/e22090937</t>
+  </si>
+  <si>
+    <t>Input data can be either a matrix, array, object from the raster package (RasterLayer, RasterStack, RasterBrick), or from the stars package [43,44]</t>
+  </si>
+  <si>
+    <t>Jakub Nowosad,Peichao Gao</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5014806603,https://openalex.org/A5074601006</t>
+  </si>
+  <si>
+    <t>Boltzmann constant,Entropy (arrow of time),Statistical physics,Boltzmann's entropy formula</t>
+  </si>
+  <si>
+    <t>STAR) aligner</t>
+  </si>
+  <si>
+    <t>10.1093/gigascience/giy092</t>
+  </si>
+  <si>
+    <t>We demonstrate that hot-starting from a saved container checkpoint can significantly reduce the execution time using the spliced transcripts alignment to a reference (STAR) aligner [14, 15] for RNA-seq data analyses</t>
+  </si>
+  <si>
+    <t>Pai Zhang,Ling‐Hong Hung,Wes Lloyd,Ka Yee Yeung</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5050437155,https://openalex.org/A5012172477,https://openalex.org/A5021815916,https://openalex.org/A5021881439</t>
+  </si>
+  <si>
+    <t>Computer science,Initialization,Container (type theory),Cloud computing,Operating system,Workflow,Software</t>
+  </si>
+  <si>
+    <t>STAR)</t>
+  </si>
+  <si>
+    <t>10.1002/advs.202000593</t>
+  </si>
+  <si>
+    <t>Spliced trans alignment to a reference (STAR) (v2.4.2a) software was used to perform sequence alignment on the clean reads of each sample</t>
+  </si>
+  <si>
+    <t>Ziyang Wang,Chunjie Sheng,Guangyan Kan,Chen Yao,Rong Geng,Shuai Chen</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5018192589,https://openalex.org/A5056445876,https://openalex.org/A5057171303,https://openalex.org/A5031993303,https://openalex.org/A5015853595,https://openalex.org/A5049317673</t>
+  </si>
+  <si>
+    <t>Gene knockdown,Small hairpin RNA,RNA interference,Cancer research,Carcinogenesis,Cell growth,Biology,Downregulation and upregulation</t>
+  </si>
+  <si>
+    <t>As a proof-of-concept example, we create a hot-start container for the spliced transcripts alignment to a reference (STAR) aligner and deploy this container to align RNA sequencing data</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>10.1186/s40478-016-0364-x</t>
+  </si>
+  <si>
+    <t>Reads were aligned using the Star 2.3.1 l aligner [51] to the ensemble reference, in which two mismatches were allowed</t>
+  </si>
+  <si>
+    <t>Annika Scheffold,Inge R. Holtman,Sandra Dieni,Nieske Brouwer,Sarah‐Fee Katz,Billy Michael Chelliah Jebaraj,Philipp J. Kahle,Bastian Hengerer,André Lechel,Stephan Stilgenbauer,Erik Boddeke,Bart J. L. Eggen,K. Lenhard Rudolph,Knut Biber</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5051011523,https://openalex.org/A5039953079,https://openalex.org/A5057076918,https://openalex.org/A5045617609,https://openalex.org/A5001009159,https://openalex.org/A5037750452,https://openalex.org/A5088711187,https://openalex.org/A5080369012,https://openalex.org/A5086342180,https://openalex.org/A5019866348,https://openalex.org/A5001954826,https://openalex.org/A5029380319,https://openalex.org/A5053296448,https://openalex.org/A5014763110</t>
+  </si>
+  <si>
+    <t>Telomere,Microglia,Ageing,Genetically modified mouse,Transgene</t>
+  </si>
+  <si>
+    <t>10.1186/1751-0147-53-57</t>
+  </si>
+  <si>
+    <t>The chromatogram was analysed by means of the program Star 5.5 (Varian), with the internal standard as reference peak</t>
+  </si>
+  <si>
+    <t>Katja Stoeckel,Leif Højvang Nielsen,Herbert Fuhrmann,Lisa Bachmann</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5033467199,https://openalex.org/A5056972779,https://openalex.org/A5086475980,https://openalex.org/A5063378305</t>
+  </si>
+  <si>
+    <t>Fish oil,Composition (language),Food science,Docosahexaenoic acid</t>
+  </si>
+  <si>
+    <t>10.1002/advs.201903583</t>
+  </si>
+  <si>
+    <t>After sequencing, the raw data were filtered using Fastp software to remove low‐quality sequences, undetected sequences, and linker sequences, and named” Clean Data.” The Clean Data sequences were compared with the genomic sequences using the Hisat2, MapSplice, Star, and Tophat2 algorithms, and a bam file of the genomic alignment was obtained; the chromosome distribution and genomic alignment rate data were obtained from the “Sample.bam” file</t>
+  </si>
+  <si>
+    <t>Zhixiao Liu,Liujun Wang,Huan Xu,Qingyun Du,Li Li,Ling Wang,En Song Zhang,Guosong Chen,Yue Wang</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5052288245,https://openalex.org/A5086689679,https://openalex.org/A5075740101,https://openalex.org/A5041093991,https://openalex.org/A5027475930,https://openalex.org/A5050487837,https://openalex.org/A5026085732,https://openalex.org/A5075261238,https://openalex.org/A5033632697</t>
+  </si>
+  <si>
+    <t>Metastasis,Prostate cancer,Cancer cell,CD44,Extracellular matrix,Extracellular,Cancer research,Cancer</t>
+  </si>
+  <si>
+    <t>STAR) RNA-Seq aligner</t>
+  </si>
+  <si>
+    <t>10.3390/cells10020273</t>
+  </si>
+  <si>
+    <t>A custom up-to-date version of the Mus Musculus genome was generated using the spliced transcripts alignment to a reference (STAR) RNA-Seq aligner [23] (version 2.7.6a) using the “—twopassMode Basic” parameter to increase the mapping change of the reads</t>
+  </si>
+  <si>
+    <t>Serena Silvestro,Agnese Gugliandolo,Luigi Chiricosta,Francesca Diomede,Oriana Trubiani,Placido Bramantı,Jacopo Pizzicannella,Emanuela Mazzon</t>
+  </si>
+  <si>
+    <t>https://openalex.org/A5072727932,https://openalex.org/A5009847970,https://openalex.org/A5005763426,https://openalex.org/A5026786600,https://openalex.org/A5041972310,https://openalex.org/A5086062480,https://openalex.org/A5069387858,https://openalex.org/A5040381615</t>
+  </si>
+  <si>
+    <t>Cell biology,microRNA,Biology,Angiogenesis,Heart development,Microvesicles,Transcriptome</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1212,6 +1860,14 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1221,7 +1877,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1229,18 +1885,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1460,10 +2170,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K85"/>
+  <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="I98" sqref="I98"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1472,7 +2182,9 @@
     <col min="2" max="2" width="17.109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="16" style="3" customWidth="1"/>
     <col min="4" max="4" width="30.21875" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="12.6640625" style="3"/>
+    <col min="5" max="7" width="12.6640625" style="3"/>
+    <col min="8" max="8" width="59.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="12.6640625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1510,7 +2222,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1540,7 +2252,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1570,7 +2282,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1600,7 +2312,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1630,7 +2342,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1660,7 +2372,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1690,7 +2402,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1720,7 +2432,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1750,7 +2462,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1780,7 +2492,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1810,7 +2522,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1840,7 +2552,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1870,7 +2582,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1900,7 +2612,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1930,7 +2642,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1960,7 +2672,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1990,7 +2702,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2020,7 +2732,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2050,7 +2762,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2080,7 +2792,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2110,7 +2822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2140,7 +2852,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2172,7 +2884,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2201,7 +2913,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2230,7 +2942,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2259,7 +2971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2288,7 +3000,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2317,7 +3029,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2346,7 +3058,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2375,7 +3087,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2404,7 +3116,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2433,7 +3145,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2462,7 +3174,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2491,7 +3203,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2520,7 +3232,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2549,7 +3261,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2578,7 +3290,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2607,7 +3319,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2636,7 +3348,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2665,7 +3377,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2694,7 +3406,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2723,7 +3435,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2752,7 +3464,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2781,7 +3493,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2810,7 +3522,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2842,7 +3554,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2871,7 +3583,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2900,7 +3612,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2929,7 +3641,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2958,7 +3670,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2987,7 +3699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -3016,7 +3728,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -3045,7 +3757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -3074,7 +3786,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -3103,7 +3815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -3132,7 +3844,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -3161,7 +3873,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -3190,7 +3902,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -3219,7 +3931,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -3248,7 +3960,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -3277,7 +3989,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -3306,7 +4018,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -3335,7 +4047,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -3527,7 +4239,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -3556,7 +4268,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -3588,7 +4300,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -3620,7 +4332,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -3652,7 +4364,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -3684,7 +4396,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -3716,7 +4428,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -3748,7 +4460,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -3780,7 +4492,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -3812,7 +4524,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -3844,7 +4556,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -3877,7 +4589,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -3909,7 +4621,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -3942,7 +4654,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -3974,7 +4686,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -4006,7 +4718,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -4035,6 +4747,1564 @@
       <c r="K85" s="3" t="s">
         <v>380</v>
       </c>
+    </row>
+    <row r="86" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="2">
+        <v>85</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="F86" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="G86" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="H86" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I86" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J86" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K86" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="2">
+        <v>86</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="H87" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I87" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J87" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K87" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="2">
+        <v>87</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="E88" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="G88" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="H88" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I88" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J88" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K88" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="2">
+        <v>88</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="H89" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I89" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J89" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K89" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="2">
+        <v>89</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="F90" s="7" t="s">
+        <v>409</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H90" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I90" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J90" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K90" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="2">
+        <v>90</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="F91" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="H91" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I91" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J91" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K91" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="2">
+        <v>91</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="F92" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="G92" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="H92" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I92" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J92" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K92" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="2">
+        <v>92</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="F93" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="H93" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I93" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J93" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K93" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="2">
+        <v>93</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>422</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="G94" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="H94" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I94" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J94" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K94" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="2">
+        <v>94</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="F95" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="G95" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="H95" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I95" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J95" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K95" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="2">
+        <v>95</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="G96" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="H96" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I96" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J96" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K96" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="2">
+        <v>96</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>441</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="H97" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I97" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J97" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K97" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="2">
+        <v>97</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>447</v>
+      </c>
+      <c r="G98" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="H98" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I98" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J98" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K98" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="2">
+        <v>98</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>450</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>451</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>452</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="H99" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I99" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J99" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K99" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="2">
+        <v>99</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>458</v>
+      </c>
+      <c r="F100" s="7" t="s">
+        <v>457</v>
+      </c>
+      <c r="G100" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="H100" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I100" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J100" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K100" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="2">
+        <v>100</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>460</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>462</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>463</v>
+      </c>
+      <c r="G101" s="7" t="s">
+        <v>465</v>
+      </c>
+      <c r="H101" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I101" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J101" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K101" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="2">
+        <v>101</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>468</v>
+      </c>
+      <c r="E102" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="G102" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="H102" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="I102" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J102" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K102" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="2">
+        <v>102</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>474</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="F103" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="G103" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="H103" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="I103" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J103" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K103" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="2">
+        <v>103</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="G104" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="H104" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="I104" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J104" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K104" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="2">
+        <v>104</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>483</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="F105" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="G105" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="H105" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="I105" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J105" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K105" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="2">
+        <v>105</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>466</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>491</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="G106" s="7" t="s">
+        <v>492</v>
+      </c>
+      <c r="H106" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="I106" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J106" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K106" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="2">
+        <v>106</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>494</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="G107" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="H107" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I107" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J107" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K107" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="2">
+        <v>107</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>499</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>500</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>501</v>
+      </c>
+      <c r="G108" s="7" t="s">
+        <v>503</v>
+      </c>
+      <c r="H108" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="I108" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J108" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K108" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="2">
+        <v>108</v>
+      </c>
+      <c r="B109" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>504</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>505</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="G109" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="H109" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="I109" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J109" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K109" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="2">
+        <v>109</v>
+      </c>
+      <c r="B110" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="E110" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="G110" s="7" t="s">
+        <v>513</v>
+      </c>
+      <c r="H110" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="I110" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J110" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K110" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="2">
+        <v>110</v>
+      </c>
+      <c r="B111" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>515</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>517</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="G111" s="7" t="s">
+        <v>518</v>
+      </c>
+      <c r="H111" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="I111" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J111" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K111" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="2">
+        <v>111</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>519</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>520</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>522</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="G112" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="H112" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="I112" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J112" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K112" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="2">
+        <v>112</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>525</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>526</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>528</v>
+      </c>
+      <c r="F113" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="G113" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="H113" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="I113" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J113" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K113" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="2">
+        <v>113</v>
+      </c>
+      <c r="B114" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="D114" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="F114" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="G114" s="7" t="s">
+        <v>534</v>
+      </c>
+      <c r="H114" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="I114" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J114" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K114" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="2">
+        <v>114</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="D115" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="E115" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="F115" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="G115" s="7" t="s">
+        <v>540</v>
+      </c>
+      <c r="H115" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="I115" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J115" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K115" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="2">
+        <v>115</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>542</v>
+      </c>
+      <c r="D116" s="7" t="s">
+        <v>543</v>
+      </c>
+      <c r="E116" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="F116" s="7" t="s">
+        <v>544</v>
+      </c>
+      <c r="G116" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="H116" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="I116" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J116" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K116" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="2">
+        <v>116</v>
+      </c>
+      <c r="B117" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>547</v>
+      </c>
+      <c r="D117" s="7" t="s">
+        <v>548</v>
+      </c>
+      <c r="E117" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="F117" s="7" t="s">
+        <v>549</v>
+      </c>
+      <c r="G117" s="7" t="s">
+        <v>551</v>
+      </c>
+      <c r="H117" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="I117" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J117" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K117" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="2">
+        <v>117</v>
+      </c>
+      <c r="B118" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="D118" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>555</v>
+      </c>
+      <c r="F118" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="G118" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="H118" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="I118" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J118" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K118" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="2">
+        <v>118</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="D119" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="E119" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="F119" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="G119" s="7" t="s">
+        <v>561</v>
+      </c>
+      <c r="H119" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="I119" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J119" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K119" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="2">
+        <v>119</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="F120" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="G120" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="H120" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I120" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J120" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K120" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="2">
+        <v>120</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="D121" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="F121" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="G121" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="H121" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I121" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J121" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K121" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="2">
+        <v>121</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>568</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>563</v>
+      </c>
+      <c r="D122" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="E122" s="7" t="s">
+        <v>566</v>
+      </c>
+      <c r="F122" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="G122" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="H122" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I122" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J122" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K122" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="2">
+        <v>122</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="E123" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="G123" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="H123" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I123" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J123" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K123" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="2">
+        <v>123</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="D124" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="E124" s="7" t="s">
+        <v>584</v>
+      </c>
+      <c r="F124" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="G124" s="7" t="s">
+        <v>585</v>
+      </c>
+      <c r="H124" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I124" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J124" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K124" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="2">
+        <v>124</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>575</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>586</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="E125" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="G125" s="7" t="s">
+        <v>590</v>
+      </c>
+      <c r="H125" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I125" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J125" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K125" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="2">
+        <v>125</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>591</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="D126" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="E126" s="11" t="s">
+        <v>595</v>
+      </c>
+      <c r="F126" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="G126" s="7" t="s">
+        <v>596</v>
+      </c>
+      <c r="H126" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="I126" s="7" t="s">
+        <v>387</v>
+      </c>
+      <c r="J126" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="K126" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E128" s="7"/>
+    </row>
+    <row r="129" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E129" s="7"/>
+    </row>
+    <row r="130" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E130" s="7"/>
+    </row>
+    <row r="131" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E131" s="7"/>
+    </row>
+    <row r="132" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E132" s="7"/>
+    </row>
+    <row r="133" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E133" s="7"/>
+    </row>
+    <row r="134" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E134" s="7"/>
+    </row>
+    <row r="135" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E135" s="7"/>
+    </row>
+    <row r="136" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E136" s="7"/>
+    </row>
+    <row r="137" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E137" s="7"/>
+    </row>
+    <row r="138" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E138" s="7"/>
+    </row>
+    <row r="139" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E139" s="7"/>
+    </row>
+    <row r="140" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E140" s="7"/>
+    </row>
+    <row r="141" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E141" s="7"/>
+    </row>
+    <row r="142" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E142" s="7"/>
+    </row>
+    <row r="143" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E143" s="7"/>
+    </row>
+    <row r="144" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E144" s="7"/>
+    </row>
+    <row r="145" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E145" s="7"/>
+    </row>
+    <row r="146" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E146" s="7"/>
+    </row>
+    <row r="147" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E147" s="7"/>
+    </row>
+    <row r="148" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E148" s="7"/>
+    </row>
+    <row r="149" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E149" s="7"/>
+    </row>
+    <row r="150" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E150" s="7"/>
+    </row>
+    <row r="151" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E151" s="7"/>
+    </row>
+    <row r="152" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E152" s="7"/>
+    </row>
+    <row r="153" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E153" s="7"/>
+    </row>
+    <row r="154" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E154" s="7"/>
+    </row>
+    <row r="155" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E155" s="7"/>
+    </row>
+    <row r="156" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E156" s="7"/>
+    </row>
+    <row r="157" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E157" s="7"/>
+    </row>
+    <row r="158" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E158" s="7"/>
+    </row>
+    <row r="159" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E159" s="7"/>
+    </row>
+    <row r="160" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E160" s="7"/>
+    </row>
+    <row r="161" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E161" s="7"/>
+    </row>
+    <row r="162" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E162" s="7"/>
+    </row>
+    <row r="163" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E163" s="7"/>
+    </row>
+    <row r="164" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E164" s="7"/>
+    </row>
+    <row r="165" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E165" s="7"/>
+    </row>
+    <row r="166" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E166" s="7"/>
+    </row>
+    <row r="167" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E167" s="7"/>
+    </row>
+    <row r="168" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E168" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4147,6 +6417,17 @@
     <hyperlink ref="H82:H83" r:id="rId107" display="https://www.rhino3d.com/" xr:uid="{332CBF04-5D33-4F0C-8625-9FD8177182F7}"/>
     <hyperlink ref="H84" r:id="rId108" xr:uid="{E378DF0D-3339-4660-9ED7-B6770E235E48}"/>
     <hyperlink ref="H85" r:id="rId109" xr:uid="{800F4166-C89D-43F2-9101-55DAEE8DAF98}"/>
+    <hyperlink ref="H108" r:id="rId110" xr:uid="{4DB9BF32-2E40-4FD1-B764-9D657B27D0B0}"/>
+    <hyperlink ref="H86" r:id="rId111" xr:uid="{095B13C8-EA3A-484D-A940-549028A05848}"/>
+    <hyperlink ref="H87:H101" r:id="rId112" display="https://github.com/alexdobin/STAR" xr:uid="{00F43458-B8AC-4E0E-B09F-8946462A6913}"/>
+    <hyperlink ref="H102" r:id="rId113" xr:uid="{7055A736-01E1-4AF8-85CA-45B773C1EE8E}"/>
+    <hyperlink ref="H103:H106" r:id="rId114" display="https://www.dnastar.com/" xr:uid="{C78180D7-218B-4918-AC5E-8A43A35310AD}"/>
+    <hyperlink ref="H107" r:id="rId115" xr:uid="{F2695FC1-29EA-4674-8F45-902012B3C8C4}"/>
+    <hyperlink ref="H109:H114" r:id="rId116" display="https://github.com/alexdobin/STAR" xr:uid="{D975C251-4E3C-484A-8614-2D288946FC00}"/>
+    <hyperlink ref="H115" r:id="rId117" xr:uid="{34FAF9B3-4D7F-44F7-A342-C504B1D017C4}"/>
+    <hyperlink ref="H116:H119" r:id="rId118" display="https://r-spatial.github.io/stars/,https://cran.r-project.org/package=stars" xr:uid="{754556D9-B595-4BF7-8058-9F833092C4A0}"/>
+    <hyperlink ref="H120" r:id="rId119" xr:uid="{9B395F25-D6C5-4EF9-B84A-913B2BC925A9}"/>
+    <hyperlink ref="H121:H126" r:id="rId120" display="https://github.com/alexdobin/STAR" xr:uid="{548AC85C-BAD6-47C8-BBB5-DEAB57DF74AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added beggining of the preprocessing of the corpus
</commit_message>
<xml_diff>
--- a/corpus/corpus.xlsx
+++ b/corpus/corpus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MASTER\TMF\Software-Disambiguation\corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4227C67-0BFD-4952-9295-512D7BFB1B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226EC43A-73CC-4D4E-AED3-ADDC811426BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2208" yWindow="2064" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmark" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="596">
   <si>
     <t>id</t>
   </si>
@@ -2169,8 +2169,8 @@
   </sheetPr>
   <dimension ref="A1:L168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2181,7 +2181,9 @@
     <col min="4" max="4" width="30.21875" style="3" customWidth="1"/>
     <col min="5" max="7" width="12.6640625" style="3"/>
     <col min="8" max="8" width="59.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="12.6640625" style="3"/>
+    <col min="9" max="11" width="12.6640625" style="3"/>
+    <col min="12" max="12" width="59.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="12.6640625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2218,7 +2220,7 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>595</v>
       </c>
     </row>
@@ -2251,6 +2253,9 @@
       <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L2" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
@@ -2281,6 +2286,9 @@
       <c r="J3" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L3" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
@@ -2311,6 +2319,9 @@
       <c r="J4" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L4" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -2341,6 +2352,9 @@
       <c r="J5" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L5" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
@@ -2371,6 +2385,9 @@
       <c r="J6" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L6" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
@@ -2401,6 +2418,9 @@
       <c r="J7" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L7" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
@@ -2431,6 +2451,9 @@
       <c r="J8" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L8" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -2461,6 +2484,9 @@
       <c r="J9" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L9" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
@@ -2491,6 +2517,9 @@
       <c r="J10" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L10" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
@@ -2521,6 +2550,9 @@
       <c r="J11" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L11" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
@@ -2551,6 +2583,9 @@
       <c r="J12" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L12" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
@@ -2581,6 +2616,9 @@
       <c r="J13" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L13" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
@@ -2611,6 +2649,9 @@
       <c r="J14" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L14" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
@@ -2641,6 +2682,9 @@
       <c r="J15" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="L15" s="5" t="s">
+        <v>373</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
@@ -2671,8 +2715,11 @@
       <c r="J16" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L16" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2701,8 +2748,11 @@
       <c r="J17" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L17" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2731,8 +2781,11 @@
       <c r="J18" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L18" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2761,8 +2814,11 @@
       <c r="J19" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L19" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2791,8 +2847,11 @@
       <c r="J20" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L20" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2821,8 +2880,11 @@
       <c r="J21" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L21" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2851,8 +2913,11 @@
       <c r="J22" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L22" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2883,8 +2948,11 @@
       <c r="J23" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L23" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2912,8 +2980,11 @@
       <c r="J24" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L24" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2941,8 +3012,11 @@
       <c r="J25" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L25" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2970,8 +3044,11 @@
       <c r="J26" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L26" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2999,8 +3076,11 @@
       <c r="J27" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L27" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -3028,8 +3108,11 @@
       <c r="J28" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L28" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -3057,8 +3140,11 @@
       <c r="J29" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L29" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -3086,8 +3172,11 @@
       <c r="J30" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L30" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -3115,8 +3204,11 @@
       <c r="J31" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L31" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -3144,8 +3236,11 @@
       <c r="J32" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L32" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -3173,8 +3268,11 @@
       <c r="J33" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L33" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -3202,8 +3300,11 @@
       <c r="J34" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L34" s="5" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -3231,8 +3332,11 @@
       <c r="J35" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L35" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -3260,8 +3364,11 @@
       <c r="J36" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L36" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -3289,8 +3396,11 @@
       <c r="J37" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L37" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -3318,8 +3428,11 @@
       <c r="J38" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L38" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -3347,8 +3460,11 @@
       <c r="J39" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L39" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -3376,8 +3492,11 @@
       <c r="J40" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L40" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -3405,8 +3524,11 @@
       <c r="J41" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L41" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -3434,8 +3556,11 @@
       <c r="J42" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L42" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -3463,8 +3588,11 @@
       <c r="J43" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L43" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -3492,8 +3620,11 @@
       <c r="J44" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L44" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -3521,8 +3652,11 @@
       <c r="J45" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L45" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -3551,8 +3685,11 @@
         <v>17</v>
       </c>
       <c r="K46" s="2"/>
-    </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L46" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -3580,8 +3717,11 @@
       <c r="J47" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L47" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -3609,8 +3749,11 @@
       <c r="J48" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L48" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -3638,8 +3781,11 @@
       <c r="J49" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L49" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -3667,8 +3813,11 @@
       <c r="J50" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L50" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -3696,8 +3845,11 @@
       <c r="J51" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L51" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -3725,8 +3877,11 @@
       <c r="J52" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L52" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -3754,8 +3909,11 @@
       <c r="J53" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L53" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -3783,8 +3941,11 @@
       <c r="J54" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L54" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -3812,8 +3973,11 @@
       <c r="J55" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L55" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -3841,8 +4005,11 @@
       <c r="J56" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L56" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -3870,8 +4037,11 @@
       <c r="J57" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L57" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -3899,8 +4069,11 @@
       <c r="J58" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L58" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -3928,8 +4101,11 @@
       <c r="J59" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L59" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -3957,8 +4133,11 @@
       <c r="J60" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L60" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -3986,8 +4165,11 @@
       <c r="J61" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L61" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -4015,8 +4197,11 @@
       <c r="J62" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L62" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -4044,8 +4229,11 @@
       <c r="J63" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L63" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -4073,8 +4261,11 @@
       <c r="J64" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L64" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -4106,8 +4297,11 @@
         <v>17</v>
       </c>
       <c r="K65" s="2"/>
-    </row>
-    <row r="66" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L65" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -4138,8 +4332,11 @@
       <c r="J66" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L66" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -4168,8 +4365,11 @@
         <v>17</v>
       </c>
       <c r="K67" s="2"/>
-    </row>
-    <row r="68" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L67" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -4200,8 +4400,11 @@
       <c r="J68" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L68" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -4232,8 +4435,11 @@
       <c r="J69" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L69" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -4261,8 +4467,11 @@
       <c r="J70" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L70" s="5" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -4293,8 +4502,11 @@
       <c r="K71" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L71" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -4325,8 +4537,11 @@
       <c r="K72" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L72" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -4357,8 +4572,11 @@
       <c r="K73" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L73" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -4389,8 +4607,11 @@
       <c r="K74" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L74" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -4421,8 +4642,11 @@
       <c r="K75" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L75" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -4453,8 +4677,11 @@
       <c r="K76" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L76" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -4485,8 +4712,11 @@
       <c r="K77" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L77" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -4517,8 +4747,11 @@
       <c r="K78" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L78" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -4549,8 +4782,11 @@
       <c r="K79" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L79" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -4582,8 +4818,11 @@
       <c r="K80" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="81" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L80" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -4614,8 +4853,11 @@
       <c r="K81" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="82" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L81" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -4647,8 +4889,11 @@
       <c r="K82" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="83" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L82" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -4679,8 +4924,11 @@
       <c r="K83" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="84" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L83" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -4711,8 +4959,11 @@
       <c r="K84" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L84" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -4741,8 +4992,11 @@
       <c r="K85" s="3" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L85" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -4776,8 +5030,11 @@
       <c r="K86" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L86" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -4811,8 +5068,11 @@
       <c r="K87" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L87" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -4846,8 +5106,11 @@
       <c r="K88" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L88" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -4881,8 +5144,11 @@
       <c r="K89" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L89" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -4916,8 +5182,11 @@
       <c r="K90" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L90" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -4951,8 +5220,11 @@
       <c r="K91" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L91" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -4986,8 +5258,11 @@
       <c r="K92" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L92" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -5021,8 +5296,11 @@
       <c r="K93" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L93" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -5056,8 +5334,11 @@
       <c r="K94" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="95" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L94" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -5091,8 +5372,11 @@
       <c r="K95" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="96" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L95" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -5126,8 +5410,11 @@
       <c r="K96" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="97" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L96" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -5161,8 +5448,11 @@
       <c r="K97" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="98" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L97" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>97</v>
       </c>
@@ -5196,8 +5486,11 @@
       <c r="K98" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="99" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L98" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -5231,8 +5524,11 @@
       <c r="K99" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="100" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L99" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -5266,8 +5562,11 @@
       <c r="K100" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="101" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L100" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>100</v>
       </c>
@@ -5301,8 +5600,11 @@
       <c r="K101" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="102" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L101" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -5336,8 +5638,11 @@
       <c r="K102" s="9" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="103" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L102" s="8" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -5371,8 +5676,11 @@
       <c r="K103" s="9" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="104" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L103" s="8" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -5406,8 +5714,11 @@
       <c r="K104" s="9" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="105" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L104" s="8" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>104</v>
       </c>
@@ -5441,8 +5752,11 @@
       <c r="K105" s="9" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="106" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L105" s="8" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -5476,8 +5790,11 @@
       <c r="K106" s="9" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="107" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L106" s="8" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -5511,8 +5828,11 @@
       <c r="K107" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L107" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -5546,8 +5866,11 @@
       <c r="K108" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="109" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L108" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>108</v>
       </c>
@@ -5581,8 +5904,11 @@
       <c r="K109" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="110" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L109" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -5616,8 +5942,11 @@
       <c r="K110" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="111" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L110" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -5651,8 +5980,11 @@
       <c r="K111" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="112" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L111" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -5686,8 +6018,11 @@
       <c r="K112" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="113" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L112" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="2">
         <v>112</v>
       </c>
@@ -5721,8 +6056,11 @@
       <c r="K113" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="114" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L113" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -5756,8 +6094,11 @@
       <c r="K114" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="115" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L114" s="10" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -5791,8 +6132,11 @@
       <c r="K115" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="116" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L115" s="8" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -5826,8 +6170,11 @@
       <c r="K116" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="117" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L116" s="8" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="2">
         <v>116</v>
       </c>
@@ -5861,8 +6208,11 @@
       <c r="K117" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L117" s="8" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -5896,8 +6246,11 @@
       <c r="K118" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="119" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L118" s="8" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="2">
         <v>118</v>
       </c>
@@ -5931,8 +6284,11 @@
       <c r="K119" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="120" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L119" s="8" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="2">
         <v>119</v>
       </c>
@@ -5966,8 +6322,11 @@
       <c r="K120" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="121" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L120" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -6001,8 +6360,11 @@
       <c r="K121" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="122" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L121" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="2">
         <v>121</v>
       </c>
@@ -6036,8 +6398,11 @@
       <c r="K122" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="123" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L122" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -6071,8 +6436,11 @@
       <c r="K123" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="124" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L123" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -6106,8 +6474,11 @@
       <c r="K124" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="125" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L124" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -6141,8 +6512,11 @@
       <c r="K125" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="126" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L125" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="2">
         <v>125</v>
       </c>
@@ -6176,8 +6550,11 @@
       <c r="K126" s="9" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="128" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L126" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E128" s="7"/>
     </row>
     <row r="129" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6422,8 +6799,41 @@
     <hyperlink ref="H116:H119" r:id="rId118" display="https://r-spatial.github.io/stars/,https://cran.r-project.org/package=stars" xr:uid="{754556D9-B595-4BF7-8058-9F833092C4A0}"/>
     <hyperlink ref="H120" r:id="rId119" xr:uid="{9B395F25-D6C5-4EF9-B84A-913B2BC925A9}"/>
     <hyperlink ref="H121:H126" r:id="rId120" display="https://github.com/alexdobin/STAR" xr:uid="{548AC85C-BAD6-47C8-BBB5-DEAB57DF74AB}"/>
+    <hyperlink ref="L2" r:id="rId121" xr:uid="{A113C7C1-D41B-4B6B-BA7F-0813BA8252D7}"/>
+    <hyperlink ref="L35" r:id="rId122" xr:uid="{884109A0-33AF-4375-ADBE-6FFCCA7B528D}"/>
+    <hyperlink ref="L58" r:id="rId123" xr:uid="{C8DD1D32-0A50-4AE3-8C0B-362C21705091}"/>
+    <hyperlink ref="L65" r:id="rId124" xr:uid="{D0265D43-4E46-465F-8942-750AA4FD72AB}"/>
+    <hyperlink ref="L66:L68" r:id="rId125" display="https://cran.r-project.org/web/packages/activity/" xr:uid="{2FF825D7-B97C-4209-9A00-61F241DFC839}"/>
+    <hyperlink ref="L69" r:id="rId126" xr:uid="{C72D9AE4-8B43-485E-9ADF-D6D972D679A9}"/>
+    <hyperlink ref="L3:L34" r:id="rId127" display="https://github.com/scikit-learn/scikit-learn" xr:uid="{F50507CE-A746-4B2F-A712-15A620019A3A}"/>
+    <hyperlink ref="L36:L56" r:id="rId128" display="https://github.com/pandas-dev/pandas" xr:uid="{803EA7A2-2307-436F-ACB1-3B66F4E4B127}"/>
+    <hyperlink ref="L59:L64" r:id="rId129" display="https://github.com/ZaixuCui/PANDA" xr:uid="{BA6FFF82-71D0-45DD-BE37-384B5CD2DF65}"/>
+    <hyperlink ref="L57" r:id="rId130" xr:uid="{617E5A21-B705-4F16-9A9D-111E1D70439D}"/>
+    <hyperlink ref="L70" r:id="rId131" xr:uid="{D3BFEADB-CE25-4173-B7D7-A69D7F61D81E}"/>
+    <hyperlink ref="L71" r:id="rId132" xr:uid="{8B8F44DF-3A84-4351-ACEB-32FBCD78E1D0}"/>
+    <hyperlink ref="L72:L75" r:id="rId133" display="https://www.rhino3d.com/" xr:uid="{CF424946-F767-4B2A-BC2B-0F91DA46D96C}"/>
+    <hyperlink ref="L76:L77" r:id="rId134" display="https://www.rhino3d.com/" xr:uid="{A1E2C419-9BD9-4DEC-A6A4-FC31545E64EE}"/>
+    <hyperlink ref="L78" r:id="rId135" xr:uid="{C0ACD060-C7EE-406B-81D5-D76323753F9C}"/>
+    <hyperlink ref="L79" r:id="rId136" xr:uid="{8F014C50-F415-4785-A84B-87A5DD070770}"/>
+    <hyperlink ref="L80" r:id="rId137" xr:uid="{B263EDDF-6B68-4320-9A24-DB335CF7176D}"/>
+    <hyperlink ref="L81" r:id="rId138" xr:uid="{63DAB0E0-9A00-4FBC-9C4E-2926C853FD4C}"/>
+    <hyperlink ref="L82:L83" r:id="rId139" display="https://www.rhino3d.com/" xr:uid="{88B6715E-7368-41A8-91F9-BC8FA7D4C2C6}"/>
+    <hyperlink ref="L84" r:id="rId140" xr:uid="{3528AF2D-A6B0-4271-A4E4-BAF8928F9F48}"/>
+    <hyperlink ref="L85" r:id="rId141" xr:uid="{5B1777D0-05AC-4A50-BA46-5DFEE7DC9021}"/>
+    <hyperlink ref="L108" r:id="rId142" xr:uid="{B1C09F9C-C4D8-43DC-AE6B-62F8A5CC9F48}"/>
+    <hyperlink ref="L86" r:id="rId143" xr:uid="{C280687E-1D4C-4A03-950C-CC783760FA78}"/>
+    <hyperlink ref="L87:L101" r:id="rId144" display="https://github.com/alexdobin/STAR" xr:uid="{1E87F349-A785-49E0-9F33-FAC46828D92B}"/>
+    <hyperlink ref="L102" r:id="rId145" xr:uid="{56FCEF6E-8728-4772-A7D0-6E6465F0D105}"/>
+    <hyperlink ref="L103:L106" r:id="rId146" display="https://www.dnastar.com/" xr:uid="{4BBFAC2D-04E1-45D8-90B9-9EAD04D469AA}"/>
+    <hyperlink ref="L107" r:id="rId147" xr:uid="{B3BF87FD-404E-4E67-8FED-E42E8B24885B}"/>
+    <hyperlink ref="L109:L114" r:id="rId148" display="https://github.com/alexdobin/STAR" xr:uid="{7A7C54B5-70F6-4FC0-947F-8265B85E363A}"/>
+    <hyperlink ref="L115" r:id="rId149" xr:uid="{E7A080CE-00EC-43CD-80B3-0FFA5039379F}"/>
+    <hyperlink ref="L116:L119" r:id="rId150" display="https://r-spatial.github.io/stars/,https://cran.r-project.org/package=stars" xr:uid="{30189263-D419-44F2-9CA7-BC320E466FC2}"/>
+    <hyperlink ref="L120" r:id="rId151" xr:uid="{4BFC74BE-E33A-4E39-823D-EE994D3BC1A1}"/>
+    <hyperlink ref="L121:L126" r:id="rId152" display="https://github.com/alexdobin/STAR" xr:uid="{86BF1402-F220-4D69-BAB1-2BF6E4E77565}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId153"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated corpus and preprocessing
</commit_message>
<xml_diff>
--- a/corpus/corpus.xlsx
+++ b/corpus/corpus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MASTER\TMF\Software-Disambiguation\corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F678E049-A0EB-4BD9-A761-E2B1B45EDA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AED11B0-34A0-47C5-81E7-C322F743A7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="597">
   <si>
     <t>id</t>
   </si>
@@ -1809,6 +1809,9 @@
   </si>
   <si>
     <t>https://r-spatial.github.io/stars/,https://cran.r-project.org/package=stars,https://github.com/r-spatial/stars/</t>
+  </si>
+  <si>
+    <t>https://cran.r-project.org/package=activity</t>
   </si>
 </sst>
 </file>
@@ -2170,8 +2173,8 @@
   </sheetPr>
   <dimension ref="A1:L168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E104" workbookViewId="0">
-      <selection activeCell="M124" sqref="M124"/>
+    <sheetView tabSelected="1" topLeftCell="E62" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4289,7 +4292,7 @@
         <v>276</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>277</v>
+        <v>596</v>
       </c>
       <c r="I65" s="4" t="s">
         <v>277</v>
@@ -4299,7 +4302,7 @@
       </c>
       <c r="K65" s="2"/>
       <c r="L65" s="4" t="s">
-        <v>277</v>
+        <v>596</v>
       </c>
     </row>
     <row r="66" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4325,7 +4328,7 @@
         <v>282</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>277</v>
+        <v>596</v>
       </c>
       <c r="I66" s="4" t="s">
         <v>277</v>
@@ -4334,7 +4337,7 @@
         <v>17</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>277</v>
+        <v>596</v>
       </c>
     </row>
     <row r="67" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4360,14 +4363,14 @@
         <v>287</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>277</v>
+        <v>596</v>
       </c>
       <c r="J67" s="2" t="s">
         <v>17</v>
       </c>
       <c r="K67" s="2"/>
       <c r="L67" s="4" t="s">
-        <v>277</v>
+        <v>596</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4393,7 +4396,7 @@
         <v>292</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>277</v>
+        <v>596</v>
       </c>
       <c r="I68" s="4" t="s">
         <v>277</v>
@@ -4402,7 +4405,7 @@
         <v>17</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>277</v>
+        <v>596</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4428,7 +4431,7 @@
         <v>297</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>277</v>
+        <v>596</v>
       </c>
       <c r="I69" s="4" t="s">
         <v>277</v>
@@ -4437,7 +4440,7 @@
         <v>17</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>277</v>
+        <v>596</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -6771,70 +6774,64 @@
     <hyperlink ref="E85" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
     <hyperlink ref="H35" r:id="rId90" xr:uid="{8E3D3C07-A1DF-45BD-8AD4-75DDD366862A}"/>
     <hyperlink ref="H58" r:id="rId91" xr:uid="{1AE6BB3C-3C0D-4C3D-84CF-5FF277D60879}"/>
-    <hyperlink ref="H65" r:id="rId92" xr:uid="{3011F4B5-892E-4D8D-AE78-6D19F022F329}"/>
-    <hyperlink ref="H66:H68" r:id="rId93" display="https://cran.r-project.org/web/packages/activity/" xr:uid="{FBB07000-5317-4BBB-8914-C7135EAF0576}"/>
-    <hyperlink ref="H69" r:id="rId94" xr:uid="{7E55440F-85A8-40A1-89F1-A6E40AD0F257}"/>
-    <hyperlink ref="H3:H34" r:id="rId95" display="https://github.com/scikit-learn/scikit-learn" xr:uid="{4176D8A1-CB25-4320-8B5A-67B31E594D81}"/>
-    <hyperlink ref="H36:H56" r:id="rId96" display="https://github.com/pandas-dev/pandas" xr:uid="{064F4E4D-0AD3-4E88-B64E-65EECC5FB73D}"/>
-    <hyperlink ref="H59:H64" r:id="rId97" display="https://github.com/ZaixuCui/PANDA" xr:uid="{A2CB303C-6B96-4817-83E4-41C22EA12383}"/>
-    <hyperlink ref="H57" r:id="rId98" xr:uid="{359ED5F9-9062-4FEF-B150-89D117A6015A}"/>
-    <hyperlink ref="H70" r:id="rId99" xr:uid="{ADA2C313-CC44-45DA-8870-A0582B3E4113}"/>
-    <hyperlink ref="H71" r:id="rId100" xr:uid="{76FCB163-ED50-4DBC-A0E1-2F3F65C8ABE3}"/>
-    <hyperlink ref="H72:H75" r:id="rId101" display="https://www.rhino3d.com/" xr:uid="{B4809B50-A4EC-41E4-9785-1762609058CF}"/>
-    <hyperlink ref="H76:H77" r:id="rId102" display="https://www.rhino3d.com/" xr:uid="{5E36533B-8172-4B58-B3BC-99EEE2C0A335}"/>
-    <hyperlink ref="H78" r:id="rId103" xr:uid="{2E45DB8F-3A0E-490A-8509-635D8A2F3DB6}"/>
-    <hyperlink ref="H79" r:id="rId104" xr:uid="{AA689A24-9945-4EFC-8D85-A9D919ADD52D}"/>
-    <hyperlink ref="H80" r:id="rId105" xr:uid="{DEB83A23-1E9D-4EAA-83F2-F04572D375F2}"/>
-    <hyperlink ref="H81" r:id="rId106" xr:uid="{EC17B8CF-A311-41BC-9F4D-A3BC7B0DDC69}"/>
-    <hyperlink ref="H82:H83" r:id="rId107" display="https://www.rhino3d.com/" xr:uid="{332CBF04-5D33-4F0C-8625-9FD8177182F7}"/>
-    <hyperlink ref="H84" r:id="rId108" xr:uid="{E378DF0D-3339-4660-9ED7-B6770E235E48}"/>
-    <hyperlink ref="H85" r:id="rId109" xr:uid="{800F4166-C89D-43F2-9101-55DAEE8DAF98}"/>
-    <hyperlink ref="H108" r:id="rId110" xr:uid="{4DB9BF32-2E40-4FD1-B764-9D657B27D0B0}"/>
-    <hyperlink ref="H86" r:id="rId111" xr:uid="{095B13C8-EA3A-484D-A940-549028A05848}"/>
-    <hyperlink ref="H87:H101" r:id="rId112" display="https://github.com/alexdobin/STAR" xr:uid="{00F43458-B8AC-4E0E-B09F-8946462A6913}"/>
-    <hyperlink ref="H102" r:id="rId113" xr:uid="{7055A736-01E1-4AF8-85CA-45B773C1EE8E}"/>
-    <hyperlink ref="H103:H106" r:id="rId114" display="https://www.dnastar.com/" xr:uid="{C78180D7-218B-4918-AC5E-8A43A35310AD}"/>
-    <hyperlink ref="H107" r:id="rId115" xr:uid="{F2695FC1-29EA-4674-8F45-902012B3C8C4}"/>
-    <hyperlink ref="H109:H114" r:id="rId116" display="https://github.com/alexdobin/STAR" xr:uid="{D975C251-4E3C-484A-8614-2D288946FC00}"/>
-    <hyperlink ref="H115" r:id="rId117" xr:uid="{34FAF9B3-4D7F-44F7-A342-C504B1D017C4}"/>
-    <hyperlink ref="H120" r:id="rId118" xr:uid="{9B395F25-D6C5-4EF9-B84A-913B2BC925A9}"/>
-    <hyperlink ref="H121:H126" r:id="rId119" display="https://github.com/alexdobin/STAR" xr:uid="{548AC85C-BAD6-47C8-BBB5-DEAB57DF74AB}"/>
-    <hyperlink ref="L2" r:id="rId120" xr:uid="{A113C7C1-D41B-4B6B-BA7F-0813BA8252D7}"/>
-    <hyperlink ref="L35" r:id="rId121" xr:uid="{884109A0-33AF-4375-ADBE-6FFCCA7B528D}"/>
-    <hyperlink ref="L58" r:id="rId122" xr:uid="{C8DD1D32-0A50-4AE3-8C0B-362C21705091}"/>
-    <hyperlink ref="L65" r:id="rId123" xr:uid="{D0265D43-4E46-465F-8942-750AA4FD72AB}"/>
-    <hyperlink ref="L66:L68" r:id="rId124" display="https://cran.r-project.org/web/packages/activity/" xr:uid="{2FF825D7-B97C-4209-9A00-61F241DFC839}"/>
-    <hyperlink ref="L69" r:id="rId125" xr:uid="{C72D9AE4-8B43-485E-9ADF-D6D972D679A9}"/>
-    <hyperlink ref="L3:L34" r:id="rId126" display="https://github.com/scikit-learn/scikit-learn" xr:uid="{F50507CE-A746-4B2F-A712-15A620019A3A}"/>
-    <hyperlink ref="L36:L56" r:id="rId127" display="https://github.com/pandas-dev/pandas" xr:uid="{803EA7A2-2307-436F-ACB1-3B66F4E4B127}"/>
-    <hyperlink ref="L59:L64" r:id="rId128" display="https://github.com/ZaixuCui/PANDA" xr:uid="{BA6FFF82-71D0-45DD-BE37-384B5CD2DF65}"/>
-    <hyperlink ref="L57" r:id="rId129" xr:uid="{617E5A21-B705-4F16-9A9D-111E1D70439D}"/>
-    <hyperlink ref="L70" r:id="rId130" xr:uid="{D3BFEADB-CE25-4173-B7D7-A69D7F61D81E}"/>
-    <hyperlink ref="L71" r:id="rId131" xr:uid="{8B8F44DF-3A84-4351-ACEB-32FBCD78E1D0}"/>
-    <hyperlink ref="L72:L75" r:id="rId132" display="https://www.rhino3d.com/" xr:uid="{CF424946-F767-4B2A-BC2B-0F91DA46D96C}"/>
-    <hyperlink ref="L76:L77" r:id="rId133" display="https://www.rhino3d.com/" xr:uid="{A1E2C419-9BD9-4DEC-A6A4-FC31545E64EE}"/>
-    <hyperlink ref="L78" r:id="rId134" xr:uid="{C0ACD060-C7EE-406B-81D5-D76323753F9C}"/>
-    <hyperlink ref="L79" r:id="rId135" xr:uid="{8F014C50-F415-4785-A84B-87A5DD070770}"/>
-    <hyperlink ref="L80" r:id="rId136" xr:uid="{B263EDDF-6B68-4320-9A24-DB335CF7176D}"/>
-    <hyperlink ref="L81" r:id="rId137" xr:uid="{63DAB0E0-9A00-4FBC-9C4E-2926C853FD4C}"/>
-    <hyperlink ref="L82:L83" r:id="rId138" display="https://www.rhino3d.com/" xr:uid="{88B6715E-7368-41A8-91F9-BC8FA7D4C2C6}"/>
-    <hyperlink ref="L84" r:id="rId139" xr:uid="{3528AF2D-A6B0-4271-A4E4-BAF8928F9F48}"/>
-    <hyperlink ref="L85" r:id="rId140" xr:uid="{5B1777D0-05AC-4A50-BA46-5DFEE7DC9021}"/>
-    <hyperlink ref="L108" r:id="rId141" xr:uid="{B1C09F9C-C4D8-43DC-AE6B-62F8A5CC9F48}"/>
-    <hyperlink ref="L86" r:id="rId142" xr:uid="{C280687E-1D4C-4A03-950C-CC783760FA78}"/>
-    <hyperlink ref="L87:L101" r:id="rId143" display="https://github.com/alexdobin/STAR" xr:uid="{1E87F349-A785-49E0-9F33-FAC46828D92B}"/>
-    <hyperlink ref="L102" r:id="rId144" xr:uid="{56FCEF6E-8728-4772-A7D0-6E6465F0D105}"/>
-    <hyperlink ref="L103:L106" r:id="rId145" display="https://www.dnastar.com/" xr:uid="{4BBFAC2D-04E1-45D8-90B9-9EAD04D469AA}"/>
-    <hyperlink ref="L107" r:id="rId146" xr:uid="{B3BF87FD-404E-4E67-8FED-E42E8B24885B}"/>
-    <hyperlink ref="L109:L114" r:id="rId147" display="https://github.com/alexdobin/STAR" xr:uid="{7A7C54B5-70F6-4FC0-947F-8265B85E363A}"/>
-    <hyperlink ref="L120" r:id="rId148" xr:uid="{4BFC74BE-E33A-4E39-823D-EE994D3BC1A1}"/>
-    <hyperlink ref="L121:L126" r:id="rId149" display="https://github.com/alexdobin/STAR" xr:uid="{86BF1402-F220-4D69-BAB1-2BF6E4E77565}"/>
-    <hyperlink ref="H116:H119" r:id="rId150" display="https://r-spatial.github.io/stars/,https://cran.r-project.org/package=stars,https://github.com/r-spatial/stars/" xr:uid="{DE11D5C5-93F5-404F-A569-E405FE19D170}"/>
-    <hyperlink ref="L115" r:id="rId151" xr:uid="{09D1EA13-B0D6-474E-B413-0F35A82F7D62}"/>
-    <hyperlink ref="L116:L119" r:id="rId152" display="https://r-spatial.github.io/stars/,https://cran.r-project.org/package=stars,https://github.com/r-spatial/stars/" xr:uid="{B9D257A4-87C2-47CA-8865-B8F828ED1FFB}"/>
+    <hyperlink ref="H3:H34" r:id="rId92" display="https://github.com/scikit-learn/scikit-learn" xr:uid="{4176D8A1-CB25-4320-8B5A-67B31E594D81}"/>
+    <hyperlink ref="H36:H56" r:id="rId93" display="https://github.com/pandas-dev/pandas" xr:uid="{064F4E4D-0AD3-4E88-B64E-65EECC5FB73D}"/>
+    <hyperlink ref="H59:H64" r:id="rId94" display="https://github.com/ZaixuCui/PANDA" xr:uid="{A2CB303C-6B96-4817-83E4-41C22EA12383}"/>
+    <hyperlink ref="H57" r:id="rId95" xr:uid="{359ED5F9-9062-4FEF-B150-89D117A6015A}"/>
+    <hyperlink ref="H70" r:id="rId96" xr:uid="{ADA2C313-CC44-45DA-8870-A0582B3E4113}"/>
+    <hyperlink ref="H71" r:id="rId97" xr:uid="{76FCB163-ED50-4DBC-A0E1-2F3F65C8ABE3}"/>
+    <hyperlink ref="H72:H75" r:id="rId98" display="https://www.rhino3d.com/" xr:uid="{B4809B50-A4EC-41E4-9785-1762609058CF}"/>
+    <hyperlink ref="H76:H77" r:id="rId99" display="https://www.rhino3d.com/" xr:uid="{5E36533B-8172-4B58-B3BC-99EEE2C0A335}"/>
+    <hyperlink ref="H78" r:id="rId100" xr:uid="{2E45DB8F-3A0E-490A-8509-635D8A2F3DB6}"/>
+    <hyperlink ref="H79" r:id="rId101" xr:uid="{AA689A24-9945-4EFC-8D85-A9D919ADD52D}"/>
+    <hyperlink ref="H80" r:id="rId102" xr:uid="{DEB83A23-1E9D-4EAA-83F2-F04572D375F2}"/>
+    <hyperlink ref="H81" r:id="rId103" xr:uid="{EC17B8CF-A311-41BC-9F4D-A3BC7B0DDC69}"/>
+    <hyperlink ref="H82:H83" r:id="rId104" display="https://www.rhino3d.com/" xr:uid="{332CBF04-5D33-4F0C-8625-9FD8177182F7}"/>
+    <hyperlink ref="H84" r:id="rId105" xr:uid="{E378DF0D-3339-4660-9ED7-B6770E235E48}"/>
+    <hyperlink ref="H85" r:id="rId106" xr:uid="{800F4166-C89D-43F2-9101-55DAEE8DAF98}"/>
+    <hyperlink ref="H108" r:id="rId107" xr:uid="{4DB9BF32-2E40-4FD1-B764-9D657B27D0B0}"/>
+    <hyperlink ref="H86" r:id="rId108" xr:uid="{095B13C8-EA3A-484D-A940-549028A05848}"/>
+    <hyperlink ref="H87:H101" r:id="rId109" display="https://github.com/alexdobin/STAR" xr:uid="{00F43458-B8AC-4E0E-B09F-8946462A6913}"/>
+    <hyperlink ref="H102" r:id="rId110" xr:uid="{7055A736-01E1-4AF8-85CA-45B773C1EE8E}"/>
+    <hyperlink ref="H103:H106" r:id="rId111" display="https://www.dnastar.com/" xr:uid="{C78180D7-218B-4918-AC5E-8A43A35310AD}"/>
+    <hyperlink ref="H107" r:id="rId112" xr:uid="{F2695FC1-29EA-4674-8F45-902012B3C8C4}"/>
+    <hyperlink ref="H109:H114" r:id="rId113" display="https://github.com/alexdobin/STAR" xr:uid="{D975C251-4E3C-484A-8614-2D288946FC00}"/>
+    <hyperlink ref="H115" r:id="rId114" xr:uid="{34FAF9B3-4D7F-44F7-A342-C504B1D017C4}"/>
+    <hyperlink ref="H120" r:id="rId115" xr:uid="{9B395F25-D6C5-4EF9-B84A-913B2BC925A9}"/>
+    <hyperlink ref="H121:H126" r:id="rId116" display="https://github.com/alexdobin/STAR" xr:uid="{548AC85C-BAD6-47C8-BBB5-DEAB57DF74AB}"/>
+    <hyperlink ref="L2" r:id="rId117" xr:uid="{A113C7C1-D41B-4B6B-BA7F-0813BA8252D7}"/>
+    <hyperlink ref="L35" r:id="rId118" xr:uid="{884109A0-33AF-4375-ADBE-6FFCCA7B528D}"/>
+    <hyperlink ref="L58" r:id="rId119" xr:uid="{C8DD1D32-0A50-4AE3-8C0B-362C21705091}"/>
+    <hyperlink ref="L3:L34" r:id="rId120" display="https://github.com/scikit-learn/scikit-learn" xr:uid="{F50507CE-A746-4B2F-A712-15A620019A3A}"/>
+    <hyperlink ref="L36:L56" r:id="rId121" display="https://github.com/pandas-dev/pandas" xr:uid="{803EA7A2-2307-436F-ACB1-3B66F4E4B127}"/>
+    <hyperlink ref="L59:L64" r:id="rId122" display="https://github.com/ZaixuCui/PANDA" xr:uid="{BA6FFF82-71D0-45DD-BE37-384B5CD2DF65}"/>
+    <hyperlink ref="L57" r:id="rId123" xr:uid="{617E5A21-B705-4F16-9A9D-111E1D70439D}"/>
+    <hyperlink ref="L70" r:id="rId124" xr:uid="{D3BFEADB-CE25-4173-B7D7-A69D7F61D81E}"/>
+    <hyperlink ref="L71" r:id="rId125" xr:uid="{8B8F44DF-3A84-4351-ACEB-32FBCD78E1D0}"/>
+    <hyperlink ref="L72:L75" r:id="rId126" display="https://www.rhino3d.com/" xr:uid="{CF424946-F767-4B2A-BC2B-0F91DA46D96C}"/>
+    <hyperlink ref="L76:L77" r:id="rId127" display="https://www.rhino3d.com/" xr:uid="{A1E2C419-9BD9-4DEC-A6A4-FC31545E64EE}"/>
+    <hyperlink ref="L78" r:id="rId128" xr:uid="{C0ACD060-C7EE-406B-81D5-D76323753F9C}"/>
+    <hyperlink ref="L79" r:id="rId129" xr:uid="{8F014C50-F415-4785-A84B-87A5DD070770}"/>
+    <hyperlink ref="L80" r:id="rId130" xr:uid="{B263EDDF-6B68-4320-9A24-DB335CF7176D}"/>
+    <hyperlink ref="L81" r:id="rId131" xr:uid="{63DAB0E0-9A00-4FBC-9C4E-2926C853FD4C}"/>
+    <hyperlink ref="L82:L83" r:id="rId132" display="https://www.rhino3d.com/" xr:uid="{88B6715E-7368-41A8-91F9-BC8FA7D4C2C6}"/>
+    <hyperlink ref="L84" r:id="rId133" xr:uid="{3528AF2D-A6B0-4271-A4E4-BAF8928F9F48}"/>
+    <hyperlink ref="L85" r:id="rId134" xr:uid="{5B1777D0-05AC-4A50-BA46-5DFEE7DC9021}"/>
+    <hyperlink ref="L108" r:id="rId135" xr:uid="{B1C09F9C-C4D8-43DC-AE6B-62F8A5CC9F48}"/>
+    <hyperlink ref="L86" r:id="rId136" xr:uid="{C280687E-1D4C-4A03-950C-CC783760FA78}"/>
+    <hyperlink ref="L87:L101" r:id="rId137" display="https://github.com/alexdobin/STAR" xr:uid="{1E87F349-A785-49E0-9F33-FAC46828D92B}"/>
+    <hyperlink ref="L102" r:id="rId138" xr:uid="{56FCEF6E-8728-4772-A7D0-6E6465F0D105}"/>
+    <hyperlink ref="L103:L106" r:id="rId139" display="https://www.dnastar.com/" xr:uid="{4BBFAC2D-04E1-45D8-90B9-9EAD04D469AA}"/>
+    <hyperlink ref="L107" r:id="rId140" xr:uid="{B3BF87FD-404E-4E67-8FED-E42E8B24885B}"/>
+    <hyperlink ref="L109:L114" r:id="rId141" display="https://github.com/alexdobin/STAR" xr:uid="{7A7C54B5-70F6-4FC0-947F-8265B85E363A}"/>
+    <hyperlink ref="L120" r:id="rId142" xr:uid="{4BFC74BE-E33A-4E39-823D-EE994D3BC1A1}"/>
+    <hyperlink ref="L121:L126" r:id="rId143" display="https://github.com/alexdobin/STAR" xr:uid="{86BF1402-F220-4D69-BAB1-2BF6E4E77565}"/>
+    <hyperlink ref="H116:H119" r:id="rId144" display="https://r-spatial.github.io/stars/,https://cran.r-project.org/package=stars,https://github.com/r-spatial/stars/" xr:uid="{DE11D5C5-93F5-404F-A569-E405FE19D170}"/>
+    <hyperlink ref="L115" r:id="rId145" xr:uid="{09D1EA13-B0D6-474E-B413-0F35A82F7D62}"/>
+    <hyperlink ref="L116:L119" r:id="rId146" display="https://r-spatial.github.io/stars/,https://cran.r-project.org/package=stars,https://github.com/r-spatial/stars/" xr:uid="{B9D257A4-87C2-47CA-8865-B8F828ED1FFB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId153"/>
+  <pageSetup orientation="portrait" r:id="rId147"/>
 </worksheet>
 </file>
 

</xml_diff>